<commit_message>
L1T fix from earlier change
</commit_message>
<xml_diff>
--- a/experimental_table.xlsx
+++ b/experimental_table.xlsx
@@ -493,19 +493,19 @@
         <v>400</v>
       </c>
       <c r="C2" t="n">
-        <v>322354.0335760382</v>
+        <v>322360.0138707894</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2614770459081837</v>
+        <v>0.2634730538922156</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2625250501002004</v>
+        <v>0.2645290581162325</v>
       </c>
       <c r="F2" t="n">
-        <v>0.262</v>
+        <v>0.264</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0008143965102210355</v>
+        <v>0.0008205980537835252</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -525,19 +525,19 @@
         <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>51613695.51154941</v>
+        <v>51391070.5775004</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4480415667466027</v>
+        <v>0.4445336544894955</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4482804585443881</v>
+        <v>0.4428152492668622</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4481609808102345</v>
+        <v>0.4436727879799666</v>
       </c>
       <c r="G3" t="n">
-        <v>6.517449077462189e-05</v>
+        <v>6.451639764099181e-05</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -557,19 +557,19 @@
         <v>53</v>
       </c>
       <c r="C4" t="n">
-        <v>25853638.76903643</v>
+        <v>25881672.87276903</v>
       </c>
       <c r="D4" t="n">
-        <v>0.442238507661559</v>
+        <v>0.4438381687516635</v>
       </c>
       <c r="E4" t="n">
-        <v>0.442415355905092</v>
+        <v>0.4445481205011997</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4423269141067502</v>
+        <v>0.4441928609483218</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001284021765766662</v>
+        <v>0.000128958633144512</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -589,19 +589,19 @@
         <v>53</v>
       </c>
       <c r="C5" t="n">
-        <v>51596676.09625827</v>
+        <v>51651234.30294618</v>
       </c>
       <c r="D5" t="n">
-        <v>0.839818763326226</v>
+        <v>0.8387912673056444</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8400426552919221</v>
+        <v>0.8399093575046654</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8399306943889111</v>
+        <v>0.8393499400559479</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0001221559295590257</v>
+        <v>0.0001220725280778166</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -621,19 +621,19 @@
         <v>53</v>
       </c>
       <c r="C6" t="n">
-        <v>40846128.08469049</v>
+        <v>40669995.20361029</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4480415667466027</v>
+        <v>0.4445336544894955</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4482804585443881</v>
+        <v>0.4428152492668622</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4481609808102345</v>
+        <v>0.4436727879799666</v>
       </c>
       <c r="G6" t="n">
-        <v>8.235532912659205e-05</v>
+        <v>8.152365713286255e-05</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -653,19 +653,19 @@
         <v>53</v>
       </c>
       <c r="C7" t="n">
-        <v>25819085.10657962</v>
+        <v>25873986.65569574</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8398932621747832</v>
+        <v>0.8386366662228731</v>
       </c>
       <c r="E7" t="n">
-        <v>0.839109570781125</v>
+        <v>0.839642761930152</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8395012335800494</v>
+        <v>0.8391394125091587</v>
       </c>
       <c r="G7" t="n">
-        <v>0.000243698090761513</v>
+        <v>0.00024359509074605</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -685,19 +685,19 @@
         <v>53</v>
       </c>
       <c r="C8" t="n">
-        <v>40832662.93237583</v>
+        <v>40875827.43311323</v>
       </c>
       <c r="D8" t="n">
-        <v>0.839818763326226</v>
+        <v>0.8387912673056444</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8400426552919221</v>
+        <v>0.8399093575046654</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8399306943889111</v>
+        <v>0.8393499400559479</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0001543577978524866</v>
+        <v>0.0001542524554400209</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -717,19 +717,19 @@
         <v>53</v>
       </c>
       <c r="C9" t="n">
-        <v>20465704.53910785</v>
+        <v>20487884.13131923</v>
       </c>
       <c r="D9" t="n">
-        <v>0.442238507661559</v>
+        <v>0.4438381687516635</v>
       </c>
       <c r="E9" t="n">
-        <v>0.442415355905092</v>
+        <v>0.4445481205011997</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4423269141067502</v>
+        <v>0.4441928609483218</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0001622061671039775</v>
+        <v>0.0001629092167728291</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -749,19 +749,19 @@
         <v>53</v>
       </c>
       <c r="C10" t="n">
-        <v>20438366.90245336</v>
+        <v>20481803.0679683</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8398932621747832</v>
+        <v>0.8386366662228731</v>
       </c>
       <c r="E10" t="n">
-        <v>0.839109570781125</v>
+        <v>0.839642761930152</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8395012335800494</v>
+        <v>0.8391394125091587</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0003078554062422273</v>
+        <v>0.0003077256482957434</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
updated with parallel processing & hlt run
</commit_message>
<xml_diff>
--- a/experimental_table.xlsx
+++ b/experimental_table.xlsx
@@ -493,19 +493,19 @@
         <v>400</v>
       </c>
       <c r="C2" t="n">
-        <v>274457.8430636273</v>
+        <v>322398.8857866722</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2909738717339668</v>
+        <v>0.2754491017964072</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2454909819639279</v>
+        <v>0.2765531062124248</v>
       </c>
       <c r="F2" t="n">
-        <v>0.266304347826087</v>
+        <v>0.276</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0008169861657682073</v>
+        <v>0.0008577945278104697</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -525,19 +525,19 @@
         <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>51659606.78187535</v>
+        <v>51678890.85532195</v>
       </c>
       <c r="D3" t="n">
-        <v>0.370925341745531</v>
+        <v>0.4037209302325581</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3761663556384964</v>
+        <v>0.4049586776859504</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3735274652547981</v>
+        <v>0.4043388567245624</v>
       </c>
       <c r="G3" t="n">
-        <v>5.501003845533609e-05</v>
+        <v>5.887606809074921e-05</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -557,19 +557,19 @@
         <v>53</v>
       </c>
       <c r="C4" t="n">
-        <v>25877246.43466898</v>
+        <v>25880917.99959877</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3727030625832224</v>
+        <v>0.3803761673023807</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3731005065315916</v>
+        <v>0.3854972007464676</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3729016786570744</v>
+        <v>0.3829195630585899</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001082221639688323</v>
+        <v>0.0001124897284547477</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -589,19 +589,19 @@
         <v>53</v>
       </c>
       <c r="C5" t="n">
-        <v>51650479.00278904</v>
+        <v>51652880.93814024</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7921887496667556</v>
+        <v>0.7931218341775527</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8840461137969505</v>
+        <v>0.8846268212905145</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0001017199870307413</v>
+        <v>0.000101901955729869</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -621,19 +621,19 @@
         <v>53</v>
       </c>
       <c r="C6" t="n">
-        <v>40882451.44169176</v>
+        <v>40897708.30791894</v>
       </c>
       <c r="D6" t="n">
-        <v>0.370925341745531</v>
+        <v>0.4037209302325581</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3761663556384964</v>
+        <v>0.4049586776859504</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3735274652547981</v>
+        <v>0.4043388567245624</v>
       </c>
       <c r="G6" t="n">
-        <v>6.951141273197847e-05</v>
+        <v>7.439658657507687e-05</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -653,19 +653,19 @@
         <v>53</v>
       </c>
       <c r="C7" t="n">
-        <v>26011000.42288958</v>
+        <v>26011411.68620238</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7537058152793614</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7929885363902959</v>
+        <v>0.795921087709944</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7728483273790191</v>
+        <v>0.8863653232390707</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0002345196935460637</v>
+        <v>0.0002034679012776482</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -685,19 +685,19 @@
         <v>53</v>
       </c>
       <c r="C8" t="n">
-        <v>40875229.81925765</v>
+        <v>40877130.14475385</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7921887496667556</v>
+        <v>0.7931218341775527</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8840461137969505</v>
+        <v>0.8846268212905145</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0001285347159521046</v>
+        <v>0.0001287646556409264</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -717,19 +717,19 @@
         <v>53</v>
       </c>
       <c r="C9" t="n">
-        <v>20484382.08983687</v>
+        <v>20487286.90503867</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3727030625832224</v>
+        <v>0.3803761673023807</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3731005065315916</v>
+        <v>0.3854972007464676</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3729016786570744</v>
+        <v>0.3829195630585899</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0001367135017513692</v>
+        <v>0.0001421045866848499</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -749,19 +749,19 @@
         <v>53</v>
       </c>
       <c r="C10" t="n">
-        <v>20590203.52902749</v>
+        <v>20590528.84795526</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7537058152793614</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7929885363902959</v>
+        <v>0.795921087709944</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7728483273790191</v>
+        <v>0.8863653232390707</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0002962618528468094</v>
+        <v>0.0002570350370377233</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
updating readme for reproducibility and re-exporting environment for system cross- compatibility
</commit_message>
<xml_diff>
--- a/experimental_table.xlsx
+++ b/experimental_table.xlsx
@@ -493,19 +493,19 @@
         <v>400</v>
       </c>
       <c r="C2" t="n">
-        <v>322398.8857866722</v>
+        <v>312785.5599425451</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2754491017964072</v>
+        <v>0.2311661506707946</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2765531062124248</v>
+        <v>0.2244488977955912</v>
       </c>
       <c r="F2" t="n">
-        <v>0.276</v>
+        <v>0.2277580071174377</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0008577945278104697</v>
+        <v>0.0007055872685981302</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -525,19 +525,19 @@
         <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>51678890.85532195</v>
+        <v>51613283.75073684</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4037209302325581</v>
+        <v>0.3906437425029988</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4049586776859504</v>
+        <v>0.3906958144494801</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4043388567245624</v>
+        <v>0.3906697767410863</v>
       </c>
       <c r="G3" t="n">
-        <v>5.887606809074921e-05</v>
+        <v>5.679149090851102e-05</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -557,19 +557,19 @@
         <v>53</v>
       </c>
       <c r="C4" t="n">
-        <v>25880917.99959877</v>
+        <v>25855353.23681396</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3803761673023807</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3854972007464676</v>
+        <v>0.3805651826179686</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3829195630585899</v>
+        <v>0.5513179492130926</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001124897284547477</v>
+        <v>6.087763453033134e-05</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -589,19 +589,19 @@
         <v>53</v>
       </c>
       <c r="C5" t="n">
-        <v>51652880.93814024</v>
+        <v>51431834.82302178</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0.7981553268279642</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7931218341775527</v>
+        <v>0.795921087709944</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8846268212905145</v>
+        <v>0.7970366415270639</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000101901955729869</v>
+        <v>0.000115932692966944</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -621,19 +621,19 @@
         <v>53</v>
       </c>
       <c r="C6" t="n">
-        <v>40897708.30791894</v>
+        <v>40845802.31418186</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4037209302325581</v>
+        <v>0.3906437425029988</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4049586776859504</v>
+        <v>0.3906958144494801</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4043388567245624</v>
+        <v>0.3906697767410863</v>
       </c>
       <c r="G6" t="n">
-        <v>7.439658657507687e-05</v>
+        <v>7.176246196223316e-05</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -653,19 +653,19 @@
         <v>53</v>
       </c>
       <c r="C7" t="n">
-        <v>26011411.68620238</v>
+        <v>25874295.03564626</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.795921087709944</v>
+        <v>0.7743268461743535</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8863653232390707</v>
+        <v>0.8728119600330554</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0002034679012776482</v>
+        <v>0.0001959537320281384</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -685,19 +685,19 @@
         <v>53</v>
       </c>
       <c r="C8" t="n">
-        <v>40877130.14475385</v>
+        <v>40702246.41595799</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>0.7981553268279642</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7931218341775527</v>
+        <v>0.795921087709944</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8846268212905145</v>
+        <v>0.7970366415270639</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0001287646556409264</v>
+        <v>0.0001464939073467507</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -717,19 +717,19 @@
         <v>53</v>
       </c>
       <c r="C9" t="n">
-        <v>20487286.90503867</v>
+        <v>20467060.82492377</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3803761673023807</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3854972007464676</v>
+        <v>0.3805651826179686</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3829195630585899</v>
+        <v>0.5513179492130926</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0001421045866848499</v>
+        <v>7.690467910695927e-05</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -749,19 +749,19 @@
         <v>53</v>
       </c>
       <c r="C10" t="n">
-        <v>20590528.84795526</v>
+        <v>20482046.99586322</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.795921087709944</v>
+        <v>0.7743268461743535</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8863653232390707</v>
+        <v>0.8728119600330554</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0002570350370377233</v>
+        <v>0.000247541892509867</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
refactoring directory into module
</commit_message>
<xml_diff>
--- a/experimental_table.xlsx
+++ b/experimental_table.xlsx
@@ -493,19 +493,19 @@
         <v>400</v>
       </c>
       <c r="C2" t="n">
-        <v>312785.5599425451</v>
+        <v>322356.9755811149</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2311661506707946</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2244488977955912</v>
+        <v>0.2204408817635271</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2277580071174377</v>
+        <v>0.361247947454844</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0007055872685981302</v>
+        <v>0.000246542046427866</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -525,19 +525,19 @@
         <v>53</v>
       </c>
       <c r="C3" t="n">
-        <v>51613283.75073684</v>
+        <v>51617607.23576894</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3906437425029988</v>
+        <v>0.394096529716793</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3906958144494801</v>
+        <v>0.3950946414289523</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3906697767410863</v>
+        <v>0.3945949544032483</v>
       </c>
       <c r="G3" t="n">
-        <v>5.679149090851102e-05</v>
+        <v>5.74948900384189e-05</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -557,19 +557,19 @@
         <v>53</v>
       </c>
       <c r="C4" t="n">
-        <v>25855353.23681396</v>
+        <v>25826015.21049996</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3805651826179686</v>
+        <v>0.3737669954678752</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5513179492130926</v>
+        <v>0.5441490393945274</v>
       </c>
       <c r="G4" t="n">
-        <v>6.087763453033134e-05</v>
+        <v>5.907972616084886e-05</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -589,19 +589,19 @@
         <v>53</v>
       </c>
       <c r="C5" t="n">
-        <v>51431834.82302178</v>
+        <v>51596401.59112387</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7981553268279642</v>
+        <v>0.7902796271637816</v>
       </c>
       <c r="E5" t="n">
-        <v>0.795921087709944</v>
+        <v>0.7911223673687017</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7970366415270639</v>
+        <v>0.7907007727151613</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000115932692966944</v>
+        <v>0.0001150887003738726</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -621,19 +621,19 @@
         <v>53</v>
       </c>
       <c r="C6" t="n">
-        <v>40845802.31418186</v>
+        <v>40849222.90134574</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3906437425029988</v>
+        <v>0.394096529716793</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3906958144494801</v>
+        <v>0.3950946414289523</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3906697767410863</v>
+        <v>0.3945949544032483</v>
       </c>
       <c r="G6" t="n">
-        <v>7.176246196223316e-05</v>
+        <v>7.265128786499048e-05</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -653,19 +653,19 @@
         <v>53</v>
       </c>
       <c r="C7" t="n">
-        <v>25874295.03564626</v>
+        <v>25846466.80855933</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7743268461743535</v>
+        <v>0.7709944014929352</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8728119600330554</v>
+        <v>0.8706909528827337</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0001959537320281384</v>
+        <v>0.0001948458374900968</v>
       </c>
       <c r="H7" t="b">
         <v>1</v>
@@ -685,19 +685,19 @@
         <v>53</v>
       </c>
       <c r="C8" t="n">
-        <v>40702246.41595799</v>
+        <v>40832445.7539193</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7981553268279642</v>
+        <v>0.7902796271637816</v>
       </c>
       <c r="E8" t="n">
-        <v>0.795921087709944</v>
+        <v>0.7911223673687017</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7970366415270639</v>
+        <v>0.7907007727151613</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0001464939073467507</v>
+        <v>0.000145427556283985</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -717,19 +717,19 @@
         <v>53</v>
       </c>
       <c r="C9" t="n">
-        <v>20467060.82492377</v>
+        <v>20443849.61398738</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3805651826179686</v>
+        <v>0.3737669954678752</v>
       </c>
       <c r="F9" t="n">
-        <v>0.5513179492130926</v>
+        <v>0.5441490393945274</v>
       </c>
       <c r="G9" t="n">
-        <v>7.690467910695927e-05</v>
+        <v>7.46333951418978e-05</v>
       </c>
       <c r="H9" t="b">
         <v>1</v>
@@ -749,19 +749,19 @@
         <v>53</v>
       </c>
       <c r="C10" t="n">
-        <v>20482046.99586322</v>
+        <v>20460030.28549328</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7743268461743535</v>
+        <v>0.7709944014929352</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8728119600330554</v>
+        <v>0.8706909528827337</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000247541892509867</v>
+        <v>0.0002461421806909273</v>
       </c>
       <c r="H10" t="b">
         <v>1</v>

</xml_diff>